<commit_message>
Binary Tree and Trie
</commit_message>
<xml_diff>
--- a/PRACTICE SHEET/FINAL450.xlsx
+++ b/PRACTICE SHEET/FINAL450.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91798\Desktop\DSA by Love Babbar\PRACTICE SHEET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E276DF31-5564-40E9-AB58-4960DEE85654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAF2C23-5EB1-46B5-890D-DE2F53EC1EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1437,7 +1437,7 @@
     <t>NO</t>
   </si>
   <si>
-    <t>Legends:  Yellow-&gt; Hard to solve revise it.</t>
+    <t>Legends:  Yellow-&gt; Hard to solve Try One more time.</t>
   </si>
 </sst>
 </file>
@@ -1895,8 +1895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1963,7 +1963,7 @@
       <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="11" t="s">

</xml_diff>